<commit_message>
Inteface funcionando e fazendo do download do arquivo ja formatado
</commit_message>
<xml_diff>
--- a/uploads/resultado.xlsx
+++ b/uploads/resultado.xlsx
@@ -75020,7 +75020,7 @@
         </is>
       </c>
       <c r="D1139" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1139" t="inlineStr"/>
       <c r="F1139" t="inlineStr"/>
@@ -75058,7 +75058,7 @@
         </is>
       </c>
       <c r="D1140" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1140" t="inlineStr"/>
       <c r="F1140" t="inlineStr"/>
@@ -75096,7 +75096,7 @@
         </is>
       </c>
       <c r="D1141" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1141" t="inlineStr"/>
       <c r="F1141" t="inlineStr"/>
@@ -75134,7 +75134,7 @@
         </is>
       </c>
       <c r="D1142" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1142" t="inlineStr"/>
       <c r="F1142" t="inlineStr"/>
@@ -75172,7 +75172,7 @@
         </is>
       </c>
       <c r="D1143" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1143" t="inlineStr"/>
       <c r="F1143" t="inlineStr"/>
@@ -75210,7 +75210,7 @@
         </is>
       </c>
       <c r="D1144" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1144" t="inlineStr"/>
       <c r="F1144" t="inlineStr"/>
@@ -75248,7 +75248,7 @@
         </is>
       </c>
       <c r="D1145" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1145" t="inlineStr"/>
       <c r="F1145" t="inlineStr"/>
@@ -75286,7 +75286,7 @@
         </is>
       </c>
       <c r="D1146" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1146" t="inlineStr"/>
       <c r="F1146" t="inlineStr"/>
@@ -75324,7 +75324,7 @@
         </is>
       </c>
       <c r="D1147" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1147" t="inlineStr"/>
       <c r="F1147" t="inlineStr"/>
@@ -75362,7 +75362,7 @@
         </is>
       </c>
       <c r="D1148" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1148" t="inlineStr"/>
       <c r="F1148" t="inlineStr"/>
@@ -75400,7 +75400,7 @@
         </is>
       </c>
       <c r="D1149" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1149" t="inlineStr"/>
       <c r="F1149" t="inlineStr"/>
@@ -75438,7 +75438,7 @@
         </is>
       </c>
       <c r="D1150" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1150" t="inlineStr"/>
       <c r="F1150" t="inlineStr"/>
@@ -75476,7 +75476,7 @@
         </is>
       </c>
       <c r="D1151" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1151" t="inlineStr"/>
       <c r="F1151" t="inlineStr"/>
@@ -75514,7 +75514,7 @@
         </is>
       </c>
       <c r="D1152" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1152" t="inlineStr"/>
       <c r="F1152" t="inlineStr"/>
@@ -75552,7 +75552,7 @@
         </is>
       </c>
       <c r="D1153" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1153" t="inlineStr"/>
       <c r="F1153" t="inlineStr"/>
@@ -75590,7 +75590,7 @@
         </is>
       </c>
       <c r="D1154" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1154" t="inlineStr"/>
       <c r="F1154" t="inlineStr"/>
@@ -75628,7 +75628,7 @@
         </is>
       </c>
       <c r="D1155" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1155" t="inlineStr"/>
       <c r="F1155" t="inlineStr"/>
@@ -75666,7 +75666,7 @@
         </is>
       </c>
       <c r="D1156" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1156" t="inlineStr"/>
       <c r="F1156" t="inlineStr"/>
@@ -75704,7 +75704,7 @@
         </is>
       </c>
       <c r="D1157" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1157" t="inlineStr"/>
       <c r="F1157" t="inlineStr"/>
@@ -75742,7 +75742,7 @@
         </is>
       </c>
       <c r="D1158" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1158" t="inlineStr"/>
       <c r="F1158" t="inlineStr"/>
@@ -75780,7 +75780,7 @@
         </is>
       </c>
       <c r="D1159" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1159" t="inlineStr"/>
       <c r="F1159" t="inlineStr"/>
@@ -75818,7 +75818,7 @@
         </is>
       </c>
       <c r="D1160" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1160" t="inlineStr"/>
       <c r="F1160" t="inlineStr"/>
@@ -75856,7 +75856,7 @@
         </is>
       </c>
       <c r="D1161" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1161" t="inlineStr"/>
       <c r="F1161" t="inlineStr"/>
@@ -75894,7 +75894,7 @@
         </is>
       </c>
       <c r="D1162" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1162" t="inlineStr"/>
       <c r="F1162" t="inlineStr"/>
@@ -75932,7 +75932,7 @@
         </is>
       </c>
       <c r="D1163" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1163" t="inlineStr"/>
       <c r="F1163" t="inlineStr"/>
@@ -75970,7 +75970,7 @@
         </is>
       </c>
       <c r="D1164" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1164" t="inlineStr"/>
       <c r="F1164" t="inlineStr"/>
@@ -76008,7 +76008,7 @@
         </is>
       </c>
       <c r="D1165" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1165" t="inlineStr"/>
       <c r="F1165" t="inlineStr"/>
@@ -76046,7 +76046,7 @@
         </is>
       </c>
       <c r="D1166" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1166" t="inlineStr"/>
       <c r="F1166" t="inlineStr"/>
@@ -76084,7 +76084,7 @@
         </is>
       </c>
       <c r="D1167" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1167" t="inlineStr"/>
       <c r="F1167" t="inlineStr"/>
@@ -76122,7 +76122,7 @@
         </is>
       </c>
       <c r="D1168" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1168" t="inlineStr"/>
       <c r="F1168" t="inlineStr"/>
@@ -76160,7 +76160,7 @@
         </is>
       </c>
       <c r="D1169" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1169" t="inlineStr"/>
       <c r="F1169" t="inlineStr"/>
@@ -76194,7 +76194,7 @@
         </is>
       </c>
       <c r="D1170" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1170" t="inlineStr"/>
       <c r="F1170" t="inlineStr"/>
@@ -76232,7 +76232,7 @@
         </is>
       </c>
       <c r="D1171" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1171" t="inlineStr"/>
       <c r="F1171" t="inlineStr"/>
@@ -76270,7 +76270,7 @@
         </is>
       </c>
       <c r="D1172" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1172" t="inlineStr"/>
       <c r="F1172" t="inlineStr"/>
@@ -76308,7 +76308,7 @@
         </is>
       </c>
       <c r="D1173" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1173" t="inlineStr"/>
       <c r="F1173" t="inlineStr"/>
@@ -76346,7 +76346,7 @@
         </is>
       </c>
       <c r="D1174" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1174" t="inlineStr"/>
       <c r="F1174" t="inlineStr"/>
@@ -76384,7 +76384,7 @@
         </is>
       </c>
       <c r="D1175" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1175" t="inlineStr"/>
       <c r="F1175" t="inlineStr"/>
@@ -76422,7 +76422,7 @@
         </is>
       </c>
       <c r="D1176" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1176" t="inlineStr"/>
       <c r="F1176" t="inlineStr"/>
@@ -76460,7 +76460,7 @@
         </is>
       </c>
       <c r="D1177" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1177" t="inlineStr"/>
       <c r="F1177" t="inlineStr"/>
@@ -76498,7 +76498,7 @@
         </is>
       </c>
       <c r="D1178" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1178" t="inlineStr"/>
       <c r="F1178" t="inlineStr"/>
@@ -76536,7 +76536,7 @@
         </is>
       </c>
       <c r="D1179" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1179" t="inlineStr"/>
       <c r="F1179" t="inlineStr"/>
@@ -76574,7 +76574,7 @@
         </is>
       </c>
       <c r="D1180" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1180" t="inlineStr"/>
       <c r="F1180" t="inlineStr"/>
@@ -76612,7 +76612,7 @@
         </is>
       </c>
       <c r="D1181" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1181" t="inlineStr"/>
       <c r="F1181" t="inlineStr"/>
@@ -76650,7 +76650,7 @@
         </is>
       </c>
       <c r="D1182" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1182" t="inlineStr"/>
       <c r="F1182" t="inlineStr"/>
@@ -76688,7 +76688,7 @@
         </is>
       </c>
       <c r="D1183" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1183" t="inlineStr"/>
       <c r="F1183" t="inlineStr"/>
@@ -76726,7 +76726,7 @@
         </is>
       </c>
       <c r="D1184" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1184" t="inlineStr"/>
       <c r="F1184" t="inlineStr"/>
@@ -76764,7 +76764,7 @@
         </is>
       </c>
       <c r="D1185" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1185" t="inlineStr"/>
       <c r="F1185" t="inlineStr"/>
@@ -76802,7 +76802,7 @@
         </is>
       </c>
       <c r="D1186" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1186" t="inlineStr"/>
       <c r="F1186" t="inlineStr"/>
@@ -76840,7 +76840,7 @@
         </is>
       </c>
       <c r="D1187" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1187" t="inlineStr"/>
       <c r="F1187" t="inlineStr"/>
@@ -76878,7 +76878,7 @@
         </is>
       </c>
       <c r="D1188" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1188" t="inlineStr"/>
       <c r="F1188" t="inlineStr"/>
@@ -76916,7 +76916,7 @@
         </is>
       </c>
       <c r="D1189" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1189" t="inlineStr"/>
       <c r="F1189" t="inlineStr"/>
@@ -76954,7 +76954,7 @@
         </is>
       </c>
       <c r="D1190" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1190" t="inlineStr"/>
       <c r="F1190" t="inlineStr"/>
@@ -76992,7 +76992,7 @@
         </is>
       </c>
       <c r="D1191" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1191" t="inlineStr"/>
       <c r="F1191" t="inlineStr"/>
@@ -77030,7 +77030,7 @@
         </is>
       </c>
       <c r="D1192" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1192" t="inlineStr"/>
       <c r="F1192" t="inlineStr"/>
@@ -77068,7 +77068,7 @@
         </is>
       </c>
       <c r="D1193" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1193" t="inlineStr"/>
       <c r="F1193" t="inlineStr"/>
@@ -77106,7 +77106,7 @@
         </is>
       </c>
       <c r="D1194" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1194" t="inlineStr"/>
       <c r="F1194" t="inlineStr"/>
@@ -77144,7 +77144,7 @@
         </is>
       </c>
       <c r="D1195" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1195" t="inlineStr"/>
       <c r="F1195" t="inlineStr"/>
@@ -77182,7 +77182,7 @@
         </is>
       </c>
       <c r="D1196" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1196" t="inlineStr"/>
       <c r="F1196" t="inlineStr"/>
@@ -77220,7 +77220,7 @@
         </is>
       </c>
       <c r="D1197" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1197" t="inlineStr"/>
       <c r="F1197" t="inlineStr"/>
@@ -77258,7 +77258,7 @@
         </is>
       </c>
       <c r="D1198" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1198" t="inlineStr"/>
       <c r="F1198" t="inlineStr"/>
@@ -77296,7 +77296,7 @@
         </is>
       </c>
       <c r="D1199" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1199" t="inlineStr"/>
       <c r="F1199" t="inlineStr"/>
@@ -77334,7 +77334,7 @@
         </is>
       </c>
       <c r="D1200" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1200" t="inlineStr"/>
       <c r="F1200" t="inlineStr"/>
@@ -77372,7 +77372,7 @@
         </is>
       </c>
       <c r="D1201" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1201" t="inlineStr"/>
       <c r="F1201" t="inlineStr"/>
@@ -77410,7 +77410,7 @@
         </is>
       </c>
       <c r="D1202" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1202" t="inlineStr"/>
       <c r="F1202" t="inlineStr"/>
@@ -77448,7 +77448,7 @@
         </is>
       </c>
       <c r="D1203" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1203" t="inlineStr"/>
       <c r="F1203" t="inlineStr"/>
@@ -77486,7 +77486,7 @@
         </is>
       </c>
       <c r="D1204" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1204" t="inlineStr"/>
       <c r="F1204" t="inlineStr"/>
@@ -77524,7 +77524,7 @@
         </is>
       </c>
       <c r="D1205" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1205" t="inlineStr"/>
       <c r="F1205" t="inlineStr"/>
@@ -77562,7 +77562,7 @@
         </is>
       </c>
       <c r="D1206" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1206" t="inlineStr"/>
       <c r="F1206" t="inlineStr"/>
@@ -77600,7 +77600,7 @@
         </is>
       </c>
       <c r="D1207" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1207" t="inlineStr"/>
       <c r="F1207" t="inlineStr"/>
@@ -77638,7 +77638,7 @@
         </is>
       </c>
       <c r="D1208" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1208" t="inlineStr"/>
       <c r="F1208" t="inlineStr"/>
@@ -77676,7 +77676,7 @@
         </is>
       </c>
       <c r="D1209" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1209" t="inlineStr"/>
       <c r="F1209" t="inlineStr"/>
@@ -77714,7 +77714,7 @@
         </is>
       </c>
       <c r="D1210" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1210" t="inlineStr"/>
       <c r="F1210" t="inlineStr"/>
@@ -77752,7 +77752,7 @@
         </is>
       </c>
       <c r="D1211" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1211" t="inlineStr"/>
       <c r="F1211" t="inlineStr"/>
@@ -77790,7 +77790,7 @@
         </is>
       </c>
       <c r="D1212" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1212" t="inlineStr"/>
       <c r="F1212" t="inlineStr"/>
@@ -77828,7 +77828,7 @@
         </is>
       </c>
       <c r="D1213" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1213" t="inlineStr"/>
       <c r="F1213" t="inlineStr"/>
@@ -77866,7 +77866,7 @@
         </is>
       </c>
       <c r="D1214" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1214" t="inlineStr"/>
       <c r="F1214" t="inlineStr"/>
@@ -77904,7 +77904,7 @@
         </is>
       </c>
       <c r="D1215" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1215" t="inlineStr"/>
       <c r="F1215" t="inlineStr"/>
@@ -77942,7 +77942,7 @@
         </is>
       </c>
       <c r="D1216" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1216" t="inlineStr"/>
       <c r="F1216" t="inlineStr"/>
@@ -77980,7 +77980,7 @@
         </is>
       </c>
       <c r="D1217" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1217" t="inlineStr"/>
       <c r="F1217" t="inlineStr"/>
@@ -78018,7 +78018,7 @@
         </is>
       </c>
       <c r="D1218" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1218" t="inlineStr"/>
       <c r="F1218" t="inlineStr"/>
@@ -78056,7 +78056,7 @@
         </is>
       </c>
       <c r="D1219" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1219" t="inlineStr"/>
       <c r="F1219" t="inlineStr"/>
@@ -78094,7 +78094,7 @@
         </is>
       </c>
       <c r="D1220" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1220" t="inlineStr"/>
       <c r="F1220" t="inlineStr"/>
@@ -78132,7 +78132,7 @@
         </is>
       </c>
       <c r="D1221" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1221" t="inlineStr"/>
       <c r="F1221" t="inlineStr"/>
@@ -78170,7 +78170,7 @@
         </is>
       </c>
       <c r="D1222" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1222" t="inlineStr"/>
       <c r="F1222" t="inlineStr"/>
@@ -78208,7 +78208,7 @@
         </is>
       </c>
       <c r="D1223" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1223" t="inlineStr"/>
       <c r="F1223" t="inlineStr"/>
@@ -78246,7 +78246,7 @@
         </is>
       </c>
       <c r="D1224" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1224" t="inlineStr"/>
       <c r="F1224" t="inlineStr"/>
@@ -78284,7 +78284,7 @@
         </is>
       </c>
       <c r="D1225" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1225" t="inlineStr"/>
       <c r="F1225" t="inlineStr"/>
@@ -78322,7 +78322,7 @@
         </is>
       </c>
       <c r="D1226" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1226" t="inlineStr"/>
       <c r="F1226" t="inlineStr"/>
@@ -78360,7 +78360,7 @@
         </is>
       </c>
       <c r="D1227" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1227" t="inlineStr"/>
       <c r="F1227" t="inlineStr"/>
@@ -78398,7 +78398,7 @@
         </is>
       </c>
       <c r="D1228" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1228" t="inlineStr"/>
       <c r="F1228" t="inlineStr"/>
@@ -78436,7 +78436,7 @@
         </is>
       </c>
       <c r="D1229" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1229" t="inlineStr"/>
       <c r="F1229" t="inlineStr"/>
@@ -78474,7 +78474,7 @@
         </is>
       </c>
       <c r="D1230" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1230" t="inlineStr"/>
       <c r="F1230" t="inlineStr"/>
@@ -78512,7 +78512,7 @@
         </is>
       </c>
       <c r="D1231" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1231" t="inlineStr"/>
       <c r="F1231" t="inlineStr"/>
@@ -78550,7 +78550,7 @@
         </is>
       </c>
       <c r="D1232" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1232" t="inlineStr"/>
       <c r="F1232" t="inlineStr"/>
@@ -78588,7 +78588,7 @@
         </is>
       </c>
       <c r="D1233" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1233" t="inlineStr"/>
       <c r="F1233" t="inlineStr"/>
@@ -78626,7 +78626,7 @@
         </is>
       </c>
       <c r="D1234" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1234" t="inlineStr"/>
       <c r="F1234" t="inlineStr"/>
@@ -78664,7 +78664,7 @@
         </is>
       </c>
       <c r="D1235" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1235" t="inlineStr"/>
       <c r="F1235" t="inlineStr"/>
@@ -78702,7 +78702,7 @@
         </is>
       </c>
       <c r="D1236" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1236" t="inlineStr"/>
       <c r="F1236" t="inlineStr"/>
@@ -78740,7 +78740,7 @@
         </is>
       </c>
       <c r="D1237" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1237" t="inlineStr"/>
       <c r="F1237" t="inlineStr"/>
@@ -78778,7 +78778,7 @@
         </is>
       </c>
       <c r="D1238" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1238" t="inlineStr"/>
       <c r="F1238" t="inlineStr"/>
@@ -78816,7 +78816,7 @@
         </is>
       </c>
       <c r="D1239" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1239" t="inlineStr"/>
       <c r="F1239" t="inlineStr"/>
@@ -78854,7 +78854,7 @@
         </is>
       </c>
       <c r="D1240" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1240" t="inlineStr"/>
       <c r="F1240" t="inlineStr"/>
@@ -78892,7 +78892,7 @@
         </is>
       </c>
       <c r="D1241" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1241" t="inlineStr"/>
       <c r="F1241" t="inlineStr"/>
@@ -78930,7 +78930,7 @@
         </is>
       </c>
       <c r="D1242" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1242" t="inlineStr"/>
       <c r="F1242" t="inlineStr"/>
@@ -78968,7 +78968,7 @@
         </is>
       </c>
       <c r="D1243" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1243" t="inlineStr"/>
       <c r="F1243" t="inlineStr"/>
@@ -79006,7 +79006,7 @@
         </is>
       </c>
       <c r="D1244" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1244" t="inlineStr"/>
       <c r="F1244" t="inlineStr"/>
@@ -79044,7 +79044,7 @@
         </is>
       </c>
       <c r="D1245" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1245" t="inlineStr"/>
       <c r="F1245" t="inlineStr"/>
@@ -79082,7 +79082,7 @@
         </is>
       </c>
       <c r="D1246" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1246" t="inlineStr"/>
       <c r="F1246" t="inlineStr"/>
@@ -79120,7 +79120,7 @@
         </is>
       </c>
       <c r="D1247" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1247" t="inlineStr"/>
       <c r="F1247" t="inlineStr"/>
@@ -79158,7 +79158,7 @@
         </is>
       </c>
       <c r="D1248" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1248" t="inlineStr"/>
       <c r="F1248" t="inlineStr"/>
@@ -79196,7 +79196,7 @@
         </is>
       </c>
       <c r="D1249" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1249" t="inlineStr"/>
       <c r="F1249" t="inlineStr"/>
@@ -79234,7 +79234,7 @@
         </is>
       </c>
       <c r="D1250" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1250" t="inlineStr"/>
       <c r="F1250" t="inlineStr"/>
@@ -79272,7 +79272,7 @@
         </is>
       </c>
       <c r="D1251" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1251" t="inlineStr"/>
       <c r="F1251" t="inlineStr"/>
@@ -79310,7 +79310,7 @@
         </is>
       </c>
       <c r="D1252" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1252" t="inlineStr"/>
       <c r="F1252" t="inlineStr"/>
@@ -79348,7 +79348,7 @@
         </is>
       </c>
       <c r="D1253" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1253" t="inlineStr"/>
       <c r="F1253" t="inlineStr"/>
@@ -79386,7 +79386,7 @@
         </is>
       </c>
       <c r="D1254" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1254" t="inlineStr"/>
       <c r="F1254" t="inlineStr"/>
@@ -79424,7 +79424,7 @@
         </is>
       </c>
       <c r="D1255" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1255" t="inlineStr"/>
       <c r="F1255" t="inlineStr"/>
@@ -79462,7 +79462,7 @@
         </is>
       </c>
       <c r="D1256" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1256" t="inlineStr"/>
       <c r="F1256" t="inlineStr"/>
@@ -79500,7 +79500,7 @@
         </is>
       </c>
       <c r="D1257" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1257" t="inlineStr"/>
       <c r="F1257" t="inlineStr"/>
@@ -79538,7 +79538,7 @@
         </is>
       </c>
       <c r="D1258" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1258" t="inlineStr"/>
       <c r="F1258" t="inlineStr"/>
@@ -79576,7 +79576,7 @@
         </is>
       </c>
       <c r="D1259" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1259" t="inlineStr"/>
       <c r="F1259" t="inlineStr"/>
@@ -79614,7 +79614,7 @@
         </is>
       </c>
       <c r="D1260" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1260" t="inlineStr"/>
       <c r="F1260" t="inlineStr"/>
@@ -79652,7 +79652,7 @@
         </is>
       </c>
       <c r="D1261" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1261" t="inlineStr"/>
       <c r="F1261" t="inlineStr"/>
@@ -79690,7 +79690,7 @@
         </is>
       </c>
       <c r="D1262" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1262" t="inlineStr"/>
       <c r="F1262" t="inlineStr"/>
@@ -79728,7 +79728,7 @@
         </is>
       </c>
       <c r="D1263" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1263" t="inlineStr"/>
       <c r="F1263" t="inlineStr"/>
@@ -79766,7 +79766,7 @@
         </is>
       </c>
       <c r="D1264" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1264" t="inlineStr"/>
       <c r="F1264" t="inlineStr"/>
@@ -79804,7 +79804,7 @@
         </is>
       </c>
       <c r="D1265" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1265" t="inlineStr"/>
       <c r="F1265" t="inlineStr"/>
@@ -79842,7 +79842,7 @@
         </is>
       </c>
       <c r="D1266" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1266" t="inlineStr"/>
       <c r="F1266" t="inlineStr"/>
@@ -79880,7 +79880,7 @@
         </is>
       </c>
       <c r="D1267" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1267" t="inlineStr"/>
       <c r="F1267" t="inlineStr"/>
@@ -79918,7 +79918,7 @@
         </is>
       </c>
       <c r="D1268" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1268" t="inlineStr"/>
       <c r="F1268" t="inlineStr"/>
@@ -79956,7 +79956,7 @@
         </is>
       </c>
       <c r="D1269" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1269" t="inlineStr"/>
       <c r="F1269" t="inlineStr"/>
@@ -79994,7 +79994,7 @@
         </is>
       </c>
       <c r="D1270" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1270" t="inlineStr"/>
       <c r="F1270" t="inlineStr"/>
@@ -80032,7 +80032,7 @@
         </is>
       </c>
       <c r="D1271" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1271" t="inlineStr"/>
       <c r="F1271" t="inlineStr"/>
@@ -80070,7 +80070,7 @@
         </is>
       </c>
       <c r="D1272" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1272" t="inlineStr"/>
       <c r="F1272" t="inlineStr"/>
@@ -80108,7 +80108,7 @@
         </is>
       </c>
       <c r="D1273" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1273" t="inlineStr"/>
       <c r="F1273" t="inlineStr"/>
@@ -80146,7 +80146,7 @@
         </is>
       </c>
       <c r="D1274" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1274" t="inlineStr"/>
       <c r="F1274" t="inlineStr"/>
@@ -80184,7 +80184,7 @@
         </is>
       </c>
       <c r="D1275" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1275" t="inlineStr"/>
       <c r="F1275" t="inlineStr"/>
@@ -80222,7 +80222,7 @@
         </is>
       </c>
       <c r="D1276" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1276" t="inlineStr"/>
       <c r="F1276" t="inlineStr"/>
@@ -80260,7 +80260,7 @@
         </is>
       </c>
       <c r="D1277" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1277" t="inlineStr"/>
       <c r="F1277" t="inlineStr"/>
@@ -80298,7 +80298,7 @@
         </is>
       </c>
       <c r="D1278" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1278" t="inlineStr"/>
       <c r="F1278" t="inlineStr"/>
@@ -80336,7 +80336,7 @@
         </is>
       </c>
       <c r="D1279" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1279" t="inlineStr"/>
       <c r="F1279" t="inlineStr"/>
@@ -80374,7 +80374,7 @@
         </is>
       </c>
       <c r="D1280" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1280" t="inlineStr"/>
       <c r="F1280" t="inlineStr"/>
@@ -80412,7 +80412,7 @@
         </is>
       </c>
       <c r="D1281" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1281" t="inlineStr"/>
       <c r="F1281" t="inlineStr"/>
@@ -80450,7 +80450,7 @@
         </is>
       </c>
       <c r="D1282" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1282" t="inlineStr"/>
       <c r="F1282" t="inlineStr"/>
@@ -80488,7 +80488,7 @@
         </is>
       </c>
       <c r="D1283" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1283" t="inlineStr"/>
       <c r="F1283" t="inlineStr"/>
@@ -80526,7 +80526,7 @@
         </is>
       </c>
       <c r="D1284" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1284" t="inlineStr"/>
       <c r="F1284" t="inlineStr"/>
@@ -80564,7 +80564,7 @@
         </is>
       </c>
       <c r="D1285" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1285" t="inlineStr"/>
       <c r="F1285" t="inlineStr"/>
@@ -80602,7 +80602,7 @@
         </is>
       </c>
       <c r="D1286" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1286" t="inlineStr"/>
       <c r="F1286" t="inlineStr"/>
@@ -80640,7 +80640,7 @@
         </is>
       </c>
       <c r="D1287" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1287" t="inlineStr"/>
       <c r="F1287" t="inlineStr"/>
@@ -80678,7 +80678,7 @@
         </is>
       </c>
       <c r="D1288" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1288" t="inlineStr"/>
       <c r="F1288" t="inlineStr"/>
@@ -80716,7 +80716,7 @@
         </is>
       </c>
       <c r="D1289" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1289" t="inlineStr"/>
       <c r="F1289" t="inlineStr"/>
@@ -80754,7 +80754,7 @@
         </is>
       </c>
       <c r="D1290" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1290" t="inlineStr"/>
       <c r="F1290" t="inlineStr"/>
@@ -80792,7 +80792,7 @@
         </is>
       </c>
       <c r="D1291" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1291" t="inlineStr"/>
       <c r="F1291" t="inlineStr"/>
@@ -80826,7 +80826,7 @@
         </is>
       </c>
       <c r="D1292" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1292" t="inlineStr"/>
       <c r="F1292" t="inlineStr"/>
@@ -80864,7 +80864,7 @@
         </is>
       </c>
       <c r="D1293" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1293" t="inlineStr"/>
       <c r="F1293" t="inlineStr"/>
@@ -80902,7 +80902,7 @@
         </is>
       </c>
       <c r="D1294" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1294" t="inlineStr"/>
       <c r="F1294" t="inlineStr"/>
@@ -80940,7 +80940,7 @@
         </is>
       </c>
       <c r="D1295" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1295" t="inlineStr"/>
       <c r="F1295" t="inlineStr"/>
@@ -80978,7 +80978,7 @@
         </is>
       </c>
       <c r="D1296" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1296" t="inlineStr"/>
       <c r="F1296" t="inlineStr"/>
@@ -81016,7 +81016,7 @@
         </is>
       </c>
       <c r="D1297" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1297" t="inlineStr"/>
       <c r="F1297" t="inlineStr"/>
@@ -81054,7 +81054,7 @@
         </is>
       </c>
       <c r="D1298" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1298" t="inlineStr"/>
       <c r="F1298" t="inlineStr"/>
@@ -81092,7 +81092,7 @@
         </is>
       </c>
       <c r="D1299" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1299" t="inlineStr"/>
       <c r="F1299" t="inlineStr"/>
@@ -81130,7 +81130,7 @@
         </is>
       </c>
       <c r="D1300" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1300" t="inlineStr"/>
       <c r="F1300" t="inlineStr"/>
@@ -81168,7 +81168,7 @@
         </is>
       </c>
       <c r="D1301" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1301" t="inlineStr"/>
       <c r="F1301" t="inlineStr"/>
@@ -81206,7 +81206,7 @@
         </is>
       </c>
       <c r="D1302" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1302" t="inlineStr"/>
       <c r="F1302" t="inlineStr"/>
@@ -81244,7 +81244,7 @@
         </is>
       </c>
       <c r="D1303" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1303" t="inlineStr"/>
       <c r="F1303" t="inlineStr"/>
@@ -81282,7 +81282,7 @@
         </is>
       </c>
       <c r="D1304" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1304" t="inlineStr"/>
       <c r="F1304" t="inlineStr"/>
@@ -81320,7 +81320,7 @@
         </is>
       </c>
       <c r="D1305" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1305" t="inlineStr"/>
       <c r="F1305" t="inlineStr"/>
@@ -81358,7 +81358,7 @@
         </is>
       </c>
       <c r="D1306" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1306" t="inlineStr"/>
       <c r="F1306" t="inlineStr"/>
@@ -81396,7 +81396,7 @@
         </is>
       </c>
       <c r="D1307" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1307" t="inlineStr"/>
       <c r="F1307" t="inlineStr"/>
@@ -81434,7 +81434,7 @@
         </is>
       </c>
       <c r="D1308" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1308" t="inlineStr"/>
       <c r="F1308" t="inlineStr"/>
@@ -81472,7 +81472,7 @@
         </is>
       </c>
       <c r="D1309" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1309" t="inlineStr"/>
       <c r="F1309" t="inlineStr"/>
@@ -81510,7 +81510,7 @@
         </is>
       </c>
       <c r="D1310" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1310" t="inlineStr"/>
       <c r="F1310" t="inlineStr"/>
@@ -81548,7 +81548,7 @@
         </is>
       </c>
       <c r="D1311" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1311" t="inlineStr"/>
       <c r="F1311" t="inlineStr"/>
@@ -81586,7 +81586,7 @@
         </is>
       </c>
       <c r="D1312" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1312" t="inlineStr"/>
       <c r="F1312" t="inlineStr"/>
@@ -81624,7 +81624,7 @@
         </is>
       </c>
       <c r="D1313" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1313" t="inlineStr"/>
       <c r="F1313" t="inlineStr"/>
@@ -81662,7 +81662,7 @@
         </is>
       </c>
       <c r="D1314" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1314" t="inlineStr"/>
       <c r="F1314" t="inlineStr"/>
@@ -81700,7 +81700,7 @@
         </is>
       </c>
       <c r="D1315" s="2" t="n">
-        <v>45694</v>
+        <v>45783</v>
       </c>
       <c r="E1315" t="inlineStr"/>
       <c r="F1315" t="inlineStr"/>

</xml_diff>

<commit_message>
Filtro de vendedores porta a porta esta funcionando normalmente agora
</commit_message>
<xml_diff>
--- a/uploads/resultado.xlsx
+++ b/uploads/resultado.xlsx
@@ -26466,7 +26466,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O413" t="inlineStr">
@@ -26493,7 +26493,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O414" t="inlineStr">
@@ -26520,7 +26520,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O415" t="inlineStr">
@@ -26547,7 +26547,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O416" t="inlineStr">
@@ -26574,7 +26574,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O417" t="inlineStr">
@@ -26601,7 +26601,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O418" t="inlineStr">
@@ -26628,7 +26628,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O419" t="inlineStr">
@@ -26655,7 +26655,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O420" t="inlineStr">
@@ -26682,7 +26682,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O421" t="inlineStr">
@@ -26709,7 +26709,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O422" t="inlineStr">
@@ -26736,7 +26736,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O423" t="inlineStr">
@@ -26763,7 +26763,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O424" t="inlineStr">
@@ -26790,7 +26790,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O425" t="inlineStr">
@@ -26817,7 +26817,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O426" t="inlineStr">
@@ -26844,7 +26844,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O427" t="inlineStr">
@@ -26871,7 +26871,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O428" t="inlineStr">
@@ -26898,7 +26898,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O429" t="inlineStr">
@@ -26925,7 +26925,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O430" t="inlineStr">
@@ -26952,7 +26952,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O431" t="inlineStr">
@@ -26979,7 +26979,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O432" t="inlineStr">
@@ -27006,7 +27006,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O433" t="inlineStr">
@@ -27033,7 +27033,7 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O434" t="inlineStr">
@@ -27060,7 +27060,7 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>18/06/2025</t>
+          <t>20/06/2025</t>
         </is>
       </c>
       <c r="O435" t="inlineStr">

</xml_diff>

<commit_message>
css em um formato mais simples e moderno
</commit_message>
<xml_diff>
--- a/uploads/resultado.xlsx
+++ b/uploads/resultado.xlsx
@@ -26466,7 +26466,7 @@
       </c>
       <c r="D413" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O413" t="inlineStr">
@@ -26493,7 +26493,7 @@
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O414" t="inlineStr">
@@ -26520,7 +26520,7 @@
       </c>
       <c r="D415" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O415" t="inlineStr">
@@ -26547,7 +26547,7 @@
       </c>
       <c r="D416" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O416" t="inlineStr">
@@ -26574,7 +26574,7 @@
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O417" t="inlineStr">
@@ -26601,7 +26601,7 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O418" t="inlineStr">
@@ -26628,7 +26628,7 @@
       </c>
       <c r="D419" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O419" t="inlineStr">
@@ -26655,7 +26655,7 @@
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O420" t="inlineStr">
@@ -26682,7 +26682,7 @@
       </c>
       <c r="D421" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O421" t="inlineStr">
@@ -26709,7 +26709,7 @@
       </c>
       <c r="D422" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O422" t="inlineStr">
@@ -26736,7 +26736,7 @@
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O423" t="inlineStr">
@@ -26763,7 +26763,7 @@
       </c>
       <c r="D424" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O424" t="inlineStr">
@@ -26790,7 +26790,7 @@
       </c>
       <c r="D425" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O425" t="inlineStr">
@@ -26817,7 +26817,7 @@
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O426" t="inlineStr">
@@ -26844,7 +26844,7 @@
       </c>
       <c r="D427" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O427" t="inlineStr">
@@ -26871,7 +26871,7 @@
       </c>
       <c r="D428" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O428" t="inlineStr">
@@ -26898,7 +26898,7 @@
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O429" t="inlineStr">
@@ -26925,7 +26925,7 @@
       </c>
       <c r="D430" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O430" t="inlineStr">
@@ -26952,7 +26952,7 @@
       </c>
       <c r="D431" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O431" t="inlineStr">
@@ -26979,7 +26979,7 @@
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O432" t="inlineStr">
@@ -27006,7 +27006,7 @@
       </c>
       <c r="D433" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O433" t="inlineStr">
@@ -27033,7 +27033,7 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O434" t="inlineStr">
@@ -27060,7 +27060,7 @@
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>20/06/2025</t>
+          <t>24/06/2025</t>
         </is>
       </c>
       <c r="O435" t="inlineStr">

</xml_diff>